<commit_message>
P3, section 8, improving accuracy with 128 units within the hidden layer
</commit_message>
<xml_diff>
--- a/units/unit_3/project_3/part2-mnist/minigrid_search.xlsx
+++ b/units/unit_3/project_3/part2-mnist/minigrid_search.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrsay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrsay\Documents\data_science\MITx_6d86x_course\units\unit_3\project_3\part2-mnist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885A861E-6ED6-4F5A-8404-137EF1D540FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C63054-2C6A-4515-8F82-39A8BD116189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{D4BEC6CA-B04C-46DF-B96B-92E81A976B4F}"/>
+    <workbookView xWindow="12600" yWindow="3000" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{D4BEC6CA-B04C-46DF-B96B-92E81A976B4F}"/>
   </bookViews>
   <sheets>
-    <sheet name="plot" sheetId="1" r:id="rId1"/>
-    <sheet name="raw data from execution" sheetId="2" r:id="rId2"/>
+    <sheet name="raw data from execution" sheetId="2" r:id="rId1"/>
+    <sheet name="plot" sheetId="1" r:id="rId2"/>
+    <sheet name="data for 128" sheetId="3" r:id="rId3"/>
+    <sheet name="plot 128" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>method</t>
   </si>
@@ -110,6 +112,51 @@
   </si>
   <si>
     <t>Loss on test set:0.26170886608171995 Accuracy on test set: 0.9229767628205128</t>
+  </si>
+  <si>
+    <t>Train loss: 0.034722 | Train accuracy: 0.991183</t>
+  </si>
+  <si>
+    <t>Val loss:   0.072786 | Val accuracy:   0.977440</t>
+  </si>
+  <si>
+    <t>Loss on test set:0.07472524237602603 Accuracy on test set: 0.9767628205128205</t>
+  </si>
+  <si>
+    <t>Train loss: 0.065230 | Train accuracy: 0.982206</t>
+  </si>
+  <si>
+    <t>Val loss:   0.079577 | Val accuracy:   0.976815</t>
+  </si>
+  <si>
+    <t>Loss on test set:0.08367944310138671 Accuracy on test set: 0.9748597756410257</t>
+  </si>
+  <si>
+    <t>Train loss: 0.208361 | Train accuracy: 0.941483</t>
+  </si>
+  <si>
+    <t>Val loss:   0.169072 | Val accuracy:   0.955047</t>
+  </si>
+  <si>
+    <t>Loss on test set:0.1977552261430388 Accuracy on test set: 0.9427083333333334</t>
+  </si>
+  <si>
+    <t>Train loss: 0.091077 | Train accuracy: 0.977271</t>
+  </si>
+  <si>
+    <t>Val loss:   0.220872 | Val accuracy:   0.966578</t>
+  </si>
+  <si>
+    <t>Loss on test set:0.23393643983329154 Accuracy on test set: 0.9613381410256411</t>
+  </si>
+  <si>
+    <t>Train loss: 0.040299 | Train accuracy: 0.989534</t>
+  </si>
+  <si>
+    <t>Val loss:   0.075300 | Val accuracy:   0.977774</t>
+  </si>
+  <si>
+    <t>Loss on test set:0.07761583802778496 Accuracy on test set: 0.9767628205128205</t>
   </si>
 </sst>
 </file>
@@ -368,6 +415,526 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1BD7-4A5E-B6DA-C0D98F813EF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="414320392"/>
+        <c:axId val="414317112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="414320392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Method</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414317112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414317112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414320392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Minigrid search</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'plot 128'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Val. accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'plot 128'!$C$4:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>batch size</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>learning rate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>momentum</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LeakyReLU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'plot 128'!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97743999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97681499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95504699999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96657800000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97777400000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E60-448E-8C3B-5B765B7A274F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'plot 128'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'plot 128'!$E$4:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97676282051282004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97485977564102499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94270833333333304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96133814102564097</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97676282051282004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E60-448E-8C3B-5B765B7A274F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -724,7 +1291,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1252,6 +2362,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6B35EF-1BBE-46BF-8479-0FB61C01BB62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1564,91 +2717,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DFA73B-177C-4138-B693-F3E7886C764B}">
-  <dimension ref="C3:E8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0.93248699999999995</v>
-      </c>
-      <c r="E4">
-        <v>0.92047275641025605</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0.93985200000000002</v>
-      </c>
-      <c r="E5">
-        <v>0.92988782051282004</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>0.93449199999999999</v>
-      </c>
-      <c r="E6">
-        <v>0.92067307692307598</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>0.89455200000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.88331330128205099</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>0.93382399999999999</v>
-      </c>
-      <c r="E8">
-        <v>0.922976762820512</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA42364-2400-4636-BB64-7357F85F64D7}">
   <dimension ref="B2:B27"/>
   <sheetViews>
@@ -1766,4 +2834,289 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DFA73B-177C-4138-B693-F3E7886C764B}">
+  <dimension ref="C3:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.93248699999999995</v>
+      </c>
+      <c r="E4">
+        <v>0.92047275641025605</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.93985200000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.92988782051282004</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0.93449199999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.92067307692307598</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0.89455200000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.88331330128205099</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0.93382399999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.922976762820512</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281E93DF-6347-40A9-974B-F1E56A1C4B75}">
+  <dimension ref="B2:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23561115-1DFA-4384-9D80-31C273F672B6}">
+  <dimension ref="C3:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.97743999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.97676282051282004</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.97681499999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.97485977564102499</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0.95504699999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.94270833333333304</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0.96657800000000005</v>
+      </c>
+      <c r="E7">
+        <v>0.96133814102564097</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0.97777400000000003</v>
+      </c>
+      <c r="E8">
+        <v>0.97676282051282004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>